<commit_message>
Re-export des executables et nouvelles moyennes
</commit_message>
<xml_diff>
--- a/tp2/logs/donnees.xlsx
+++ b/tp2/logs/donnees.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="238">
   <si>
     <t>Nom du fichier</t>
   </si>
@@ -747,13 +747,22 @@
   </si>
   <si>
     <t>revenuLocal</t>
+  </si>
+  <si>
+    <t>Exemplaire</t>
+  </si>
+  <si>
+    <t>Temps (ns)</t>
+  </si>
+  <si>
+    <t>Temps(ns)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -771,6 +780,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -796,7 +813,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -858,38 +875,53 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1201,7 +1233,7 @@
   <dimension ref="A1:O250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,21 +1298,21 @@
       <c r="G2">
         <v>6818</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="10"/>
+      <c r="L2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="10"/>
+      <c r="N2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="6"/>
+      <c r="O2" s="10"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1304,23 +1336,23 @@
       <c r="G3">
         <v>11972</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9" t="s">
+      <c r="I3" s="4"/>
+      <c r="J3" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="6" t="s">
         <v>230</v>
       </c>
     </row>
@@ -1346,30 +1378,30 @@
       <c r="G4">
         <v>18184</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="2">
         <f>AVERAGE(B2:B11)</f>
         <v>19172238.100000001</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="2">
         <f>AVERAGE(C2:C11)</f>
         <v>27813.4</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="2">
         <f t="shared" ref="L4:O4" si="0">AVERAGE(D2:D11)</f>
         <v>1109475116.3</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="2">
         <f t="shared" si="0"/>
         <v>36469.1</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="2">
         <f t="shared" si="0"/>
         <v>220425568.90000001</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="2">
         <f t="shared" si="0"/>
         <v>32469.3</v>
       </c>
@@ -1396,30 +1428,30 @@
       <c r="G5">
         <v>24990</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="2">
         <f>AVERAGE(B13:B22)</f>
         <v>17082813</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="2">
         <f t="shared" ref="K5:O5" si="1">AVERAGE(C13:C22)</f>
         <v>2878.4</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="2">
         <f t="shared" si="1"/>
         <v>147733924.90000001</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="2">
         <f t="shared" si="1"/>
         <v>3724.7</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="2">
         <f t="shared" si="1"/>
         <v>204205342</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="2">
         <f t="shared" si="1"/>
         <v>3335.7</v>
       </c>
@@ -1446,30 +1478,30 @@
       <c r="G6">
         <v>29798</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="2">
         <f>AVERAGE(B24:B33)</f>
         <v>19567361.199999999</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="2">
         <f t="shared" ref="K6:O6" si="2">AVERAGE(C24:C33)</f>
         <v>313.89999999999998</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="2">
         <f t="shared" si="2"/>
         <v>49826671.100000001</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="2">
         <f t="shared" si="2"/>
         <v>421</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="2">
         <f t="shared" si="2"/>
         <v>187573442.09999999</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="2">
         <f t="shared" si="2"/>
         <v>360.3</v>
       </c>
@@ -1496,30 +1528,30 @@
       <c r="G7">
         <v>35324</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="2">
         <f>AVERAGE(B35:B44)</f>
         <v>1929205</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="2">
         <f t="shared" ref="K7:O7" si="3">AVERAGE(C35:C44)</f>
         <v>2859.5</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="2">
         <f t="shared" si="3"/>
         <v>52673413.100000001</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="2">
         <f t="shared" si="3"/>
         <v>3675.7</v>
       </c>
-      <c r="N7" s="10">
+      <c r="N7" s="2">
         <f t="shared" si="3"/>
         <v>24649228.399999999</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="2">
         <f t="shared" si="3"/>
         <v>3420.8</v>
       </c>
@@ -1546,30 +1578,30 @@
       <c r="G8">
         <v>40463</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="2">
         <f>AVERAGE(B46:B54)</f>
         <v>1942892.2222222222</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="2">
         <f t="shared" ref="K8:O8" si="4">AVERAGE(C46:C54)</f>
         <v>315.66666666666669</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="2">
         <f t="shared" si="4"/>
         <v>17472890.666666668</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="2">
         <f t="shared" si="4"/>
         <v>403.66666666666669</v>
       </c>
-      <c r="N8" s="10">
+      <c r="N8" s="2">
         <f t="shared" si="4"/>
         <v>25056521.111111112</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="2">
         <f t="shared" si="4"/>
         <v>369.88888888888891</v>
       </c>
@@ -1596,30 +1628,30 @@
       <c r="G9">
         <v>45928</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="2">
         <f>AVERAGE(B56:B64)</f>
         <v>1748640.888888889</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="2">
         <f t="shared" ref="K9:O9" si="5">AVERAGE(C56:C64)</f>
         <v>32.666666666666664</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="2">
         <f t="shared" si="5"/>
         <v>1926012.888888889</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="2">
         <f t="shared" si="5"/>
         <v>43.333333333333336</v>
       </c>
-      <c r="N9" s="10">
+      <c r="N9" s="2">
         <f t="shared" si="5"/>
         <v>17216338.222222224</v>
       </c>
-      <c r="O9" s="10">
+      <c r="O9" s="2">
         <f t="shared" si="5"/>
         <v>39</v>
       </c>
@@ -1646,30 +1678,30 @@
       <c r="G10">
         <v>53381</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="2">
         <f>AVERAGE(B66:B73)</f>
         <v>910659.875</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="2">
         <f t="shared" ref="K10:O10" si="6">AVERAGE(C66:C73)</f>
         <v>1004.75</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="2">
         <f t="shared" si="6"/>
         <v>9498412.5</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="2">
         <f t="shared" si="6"/>
         <v>1106.125</v>
       </c>
-      <c r="N10" s="10">
+      <c r="N10" s="2">
         <f t="shared" si="6"/>
         <v>1939351.75</v>
       </c>
-      <c r="O10" s="10">
+      <c r="O10" s="2">
         <f t="shared" si="6"/>
         <v>1069.375</v>
       </c>
@@ -1696,30 +1728,30 @@
       <c r="G11">
         <v>57835</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="2">
         <f>AVERAGE(B75:B84)</f>
         <v>955876.9</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="2">
         <f t="shared" ref="K11:O11" si="7">AVERAGE(C75:C84)</f>
         <v>89.1</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="2">
         <f t="shared" si="7"/>
         <v>918119.5</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="2">
         <f t="shared" si="7"/>
         <v>108.2</v>
       </c>
-      <c r="N11" s="10">
+      <c r="N11" s="2">
         <f t="shared" si="7"/>
         <v>1929649.1</v>
       </c>
-      <c r="O11" s="10">
+      <c r="O11" s="2">
         <f t="shared" si="7"/>
         <v>99.6</v>
       </c>
@@ -1727,13 +1759,13 @@
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="F12"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1757,31 +1789,31 @@
       <c r="G13">
         <v>664</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="2">
         <f>AVERAGE(B86:B94)</f>
         <v>914120.77777777775</v>
       </c>
-      <c r="K13" s="10">
-        <f t="shared" ref="K13:O13" si="8">AVERAGE(C86:C94)</f>
+      <c r="K13" s="2">
+        <f>AVERAGE(C86:C94)</f>
         <v>11.111111111111111</v>
       </c>
-      <c r="L13" s="10">
-        <f t="shared" si="8"/>
+      <c r="L13" s="2">
+        <f>AVERAGE(D86:D94)</f>
         <v>612259.77777777775</v>
       </c>
-      <c r="M13" s="10">
-        <f t="shared" si="8"/>
+      <c r="M13" s="2">
+        <f>AVERAGE(E86:E94)</f>
         <v>13.111111111111111</v>
       </c>
-      <c r="N13" s="10">
-        <f t="shared" si="8"/>
+      <c r="N13" s="2">
+        <f>AVERAGE(F86:F94)</f>
         <v>1918262.5555555555</v>
       </c>
-      <c r="O13" s="10">
-        <f t="shared" si="8"/>
+      <c r="O13" s="2">
+        <f>AVERAGE(G86:G94)</f>
         <v>11.333333333333334</v>
       </c>
     </row>
@@ -1807,31 +1839,31 @@
       <c r="G14">
         <v>1254</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="2">
         <f>AVERAGE(B96:B104)</f>
         <v>3114161.5555555555</v>
       </c>
-      <c r="K14" s="10">
-        <f t="shared" ref="K14:O14" si="9">AVERAGE(C96:C104)</f>
+      <c r="K14" s="2">
+        <f>AVERAGE(C96:C104)</f>
         <v>5891.1111111111113</v>
       </c>
-      <c r="L14" s="10">
-        <f t="shared" si="9"/>
+      <c r="L14" s="2">
+        <f>AVERAGE(D96:D104)</f>
         <v>77868910.222222224</v>
       </c>
-      <c r="M14" s="10">
-        <f t="shared" si="9"/>
+      <c r="M14" s="2">
+        <f>AVERAGE(E96:E104)</f>
         <v>7610.7777777777774</v>
       </c>
-      <c r="N14" s="10">
-        <f t="shared" si="9"/>
+      <c r="N14" s="2">
+        <f>AVERAGE(F96:F104)</f>
         <v>46580486.666666664</v>
       </c>
-      <c r="O14" s="10">
-        <f t="shared" si="9"/>
+      <c r="O14" s="2">
+        <f>AVERAGE(G96:G104)</f>
         <v>6884.2222222222226</v>
       </c>
     </row>
@@ -1857,31 +1889,31 @@
       <c r="G15">
         <v>1793</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="2">
         <f>AVERAGE(B106:B115)</f>
         <v>2918555.8</v>
       </c>
-      <c r="K15" s="10">
-        <f t="shared" ref="K15:O15" si="10">AVERAGE(C106:C115)</f>
+      <c r="K15" s="2">
+        <f>AVERAGE(C106:C115)</f>
         <v>574.9</v>
       </c>
-      <c r="L15" s="10">
-        <f t="shared" si="10"/>
+      <c r="L15" s="2">
+        <f>AVERAGE(D106:D115)</f>
         <v>41854789.799999997</v>
       </c>
-      <c r="M15" s="10">
-        <f t="shared" si="10"/>
+      <c r="M15" s="2">
+        <f>AVERAGE(E106:E115)</f>
         <v>741</v>
       </c>
-      <c r="N15" s="10">
-        <f t="shared" si="10"/>
+      <c r="N15" s="2">
+        <f>AVERAGE(F106:F115)</f>
         <v>45450803.700000003</v>
       </c>
-      <c r="O15" s="10">
-        <f t="shared" si="10"/>
+      <c r="O15" s="2">
+        <f>AVERAGE(G106:G115)</f>
         <v>678.5</v>
       </c>
     </row>
@@ -1907,31 +1939,31 @@
       <c r="G16">
         <v>2426</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="2">
         <f>AVERAGE(B117:B126)</f>
         <v>2724902.2</v>
       </c>
-      <c r="K16" s="10">
-        <f t="shared" ref="K16:O16" si="11">AVERAGE(C117:C126)</f>
+      <c r="K16" s="2">
+        <f>AVERAGE(C117:C126)</f>
         <v>62.5</v>
       </c>
-      <c r="L16" s="10">
-        <f t="shared" si="11"/>
+      <c r="L16" s="2">
+        <f>AVERAGE(D117:D126)</f>
         <v>9278231.3000000007</v>
       </c>
-      <c r="M16" s="10">
-        <f t="shared" si="11"/>
+      <c r="M16" s="2">
+        <f>AVERAGE(E117:E126)</f>
         <v>83.8</v>
       </c>
-      <c r="N16" s="10">
-        <f t="shared" si="11"/>
+      <c r="N16" s="2">
+        <f>AVERAGE(F117:F126)</f>
         <v>38532225.799999997</v>
       </c>
-      <c r="O16" s="10">
-        <f t="shared" si="11"/>
+      <c r="O16" s="2">
+        <f>AVERAGE(G117:G126)</f>
         <v>73.8</v>
       </c>
     </row>
@@ -1957,31 +1989,31 @@
       <c r="G17">
         <v>3015</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="2">
         <f>AVERAGE(B128:B136)</f>
         <v>1002141.7777777778</v>
       </c>
-      <c r="K17" s="10">
-        <f t="shared" ref="K17:O17" si="12">AVERAGE(C128:C136)</f>
+      <c r="K17" s="2">
+        <f>AVERAGE(C128:C136)</f>
         <v>967.11111111111109</v>
       </c>
-      <c r="L17" s="10">
-        <f t="shared" si="12"/>
+      <c r="L17" s="2">
+        <f>AVERAGE(D128:D136)</f>
         <v>12751036</v>
       </c>
-      <c r="M17" s="10">
-        <f t="shared" si="12"/>
+      <c r="M17" s="2">
+        <f>AVERAGE(E128:E136)</f>
         <v>1235.5555555555557</v>
       </c>
-      <c r="N17" s="10">
-        <f t="shared" si="12"/>
+      <c r="N17" s="2">
+        <f>AVERAGE(F128:F136)</f>
         <v>3018903.4444444445</v>
       </c>
-      <c r="O17" s="10">
-        <f t="shared" si="12"/>
+      <c r="O17" s="2">
+        <f>AVERAGE(G128:G136)</f>
         <v>1101.7777777777778</v>
       </c>
     </row>
@@ -2007,31 +2039,31 @@
       <c r="G18">
         <v>3645</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="2">
         <f>AVERAGE(B138:B147)</f>
         <v>1008420.7</v>
       </c>
-      <c r="K18" s="10">
-        <f t="shared" ref="K18:O18" si="13">AVERAGE(C138:C147)</f>
+      <c r="K18" s="2">
+        <f>AVERAGE(C138:C147)</f>
         <v>99.2</v>
       </c>
-      <c r="L18" s="10">
-        <f t="shared" si="13"/>
+      <c r="L18" s="2">
+        <f>AVERAGE(D138:D147)</f>
         <v>1267146.3</v>
       </c>
-      <c r="M18" s="10">
-        <f t="shared" si="13"/>
+      <c r="M18" s="2">
+        <f>AVERAGE(E138:E147)</f>
         <v>119.9</v>
       </c>
-      <c r="N18" s="10">
-        <f t="shared" si="13"/>
+      <c r="N18" s="2">
+        <f>AVERAGE(F138:F147)</f>
         <v>2839615.4</v>
       </c>
-      <c r="O18" s="10">
-        <f t="shared" si="13"/>
+      <c r="O18" s="2">
+        <f>AVERAGE(G138:G147)</f>
         <v>111.1</v>
       </c>
     </row>
@@ -2057,31 +2089,31 @@
       <c r="G19">
         <v>4150</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="2">
         <f>AVERAGE(B149:B158)</f>
         <v>945117.3</v>
       </c>
-      <c r="K19" s="10">
-        <f t="shared" ref="K19:O19" si="14">AVERAGE(C149:C158)</f>
+      <c r="K19" s="2">
+        <f>AVERAGE(C149:C158)</f>
         <v>11.7</v>
       </c>
-      <c r="L19" s="10">
-        <f t="shared" si="14"/>
+      <c r="L19" s="2">
+        <f>AVERAGE(D149:D158)</f>
         <v>665377.19999999995</v>
       </c>
-      <c r="M19" s="10">
-        <f t="shared" si="14"/>
+      <c r="M19" s="2">
+        <f>AVERAGE(E149:E158)</f>
         <v>13.9</v>
       </c>
-      <c r="N19" s="10">
-        <f t="shared" si="14"/>
+      <c r="N19" s="2">
+        <f>AVERAGE(F149:F158)</f>
         <v>2807340.3</v>
       </c>
-      <c r="O19" s="10">
-        <f t="shared" si="14"/>
+      <c r="O19" s="2">
+        <f>AVERAGE(G149:G158)</f>
         <v>13</v>
       </c>
     </row>
@@ -2107,31 +2139,31 @@
       <c r="G20">
         <v>4927</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="2">
         <f>AVERAGE(B160:B169)</f>
         <v>12165247.300000001</v>
       </c>
-      <c r="K20" s="10">
-        <f t="shared" ref="K20:O20" si="15">AVERAGE(C160:C169)</f>
+      <c r="K20" s="2">
+        <f>AVERAGE(C160:C169)</f>
         <v>13751.8</v>
       </c>
-      <c r="L20" s="10">
-        <f t="shared" si="15"/>
+      <c r="L20" s="2">
+        <f>AVERAGE(D160:D169)</f>
         <v>309694953.39999998</v>
       </c>
-      <c r="M20" s="10">
-        <f t="shared" si="15"/>
+      <c r="M20" s="2">
+        <f>AVERAGE(E160:E169)</f>
         <v>18027.2</v>
       </c>
-      <c r="N20" s="10">
-        <f t="shared" si="15"/>
+      <c r="N20" s="2">
+        <f>AVERAGE(F160:F169)</f>
         <v>114938772</v>
       </c>
-      <c r="O20" s="10">
-        <f t="shared" si="15"/>
+      <c r="O20" s="2">
+        <f>AVERAGE(G160:G169)</f>
         <v>16239.8</v>
       </c>
     </row>
@@ -2157,31 +2189,31 @@
       <c r="G21">
         <v>5469</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="2">
         <f>AVERAGE(B171:B180)</f>
         <v>11623733.800000001</v>
       </c>
-      <c r="K21" s="10">
-        <f t="shared" ref="K21:O21" si="16">AVERAGE(C171:C180)</f>
+      <c r="K21" s="2">
+        <f>AVERAGE(C171:C180)</f>
         <v>1429.5</v>
       </c>
-      <c r="L21" s="10">
-        <f t="shared" si="16"/>
+      <c r="L21" s="2">
+        <f>AVERAGE(D171:D180)</f>
         <v>64749464.799999997</v>
       </c>
-      <c r="M21" s="10">
-        <f t="shared" si="16"/>
+      <c r="M21" s="2">
+        <f>AVERAGE(E171:E180)</f>
         <v>1858.8</v>
       </c>
-      <c r="N21" s="10">
-        <f t="shared" si="16"/>
+      <c r="N21" s="2">
+        <f>AVERAGE(F171:F180)</f>
         <v>104298181.7</v>
       </c>
-      <c r="O21" s="10">
-        <f t="shared" si="16"/>
+      <c r="O21" s="2">
+        <f>AVERAGE(G171:G180)</f>
         <v>1676</v>
       </c>
     </row>
@@ -2207,44 +2239,44 @@
       <c r="G22">
         <v>6014</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="2">
         <f>AVERAGE(B182:B191)</f>
         <v>10681418.4</v>
       </c>
-      <c r="K22" s="10">
-        <f t="shared" ref="K22:O22" si="17">AVERAGE(C182:C191)</f>
+      <c r="K22" s="2">
+        <f>AVERAGE(C182:C191)</f>
         <v>153.80000000000001</v>
       </c>
-      <c r="L22" s="10">
-        <f t="shared" si="17"/>
+      <c r="L22" s="2">
+        <f>AVERAGE(D182:D191)</f>
         <v>34899595.200000003</v>
       </c>
-      <c r="M22" s="10">
-        <f t="shared" si="17"/>
+      <c r="M22" s="2">
+        <f>AVERAGE(E182:E191)</f>
         <v>209.5</v>
       </c>
-      <c r="N22" s="10">
-        <f t="shared" si="17"/>
+      <c r="N22" s="2">
+        <f>AVERAGE(F182:F191)</f>
         <v>98601858.200000003</v>
       </c>
-      <c r="O22" s="10">
-        <f t="shared" si="17"/>
+      <c r="O22" s="2">
+        <f>AVERAGE(G182:G191)</f>
         <v>181.6</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="F23"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -2268,31 +2300,31 @@
       <c r="G24">
         <v>67</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J24" s="2">
         <f>AVERAGE(B193:B202)</f>
         <v>1434623</v>
       </c>
-      <c r="K24" s="10">
-        <f t="shared" ref="K24:O24" si="18">AVERAGE(C193:C202)</f>
+      <c r="K24" s="2">
+        <f>AVERAGE(C193:C202)</f>
         <v>1629.1</v>
       </c>
-      <c r="L24" s="10">
-        <f t="shared" si="18"/>
+      <c r="L24" s="2">
+        <f>AVERAGE(D193:D202)</f>
         <v>34640787.899999999</v>
       </c>
-      <c r="M24" s="10">
-        <f t="shared" si="18"/>
+      <c r="M24" s="2">
+        <f>AVERAGE(E193:E202)</f>
         <v>1967.6</v>
       </c>
-      <c r="N24" s="10">
-        <f t="shared" si="18"/>
+      <c r="N24" s="2">
+        <f>AVERAGE(F193:F202)</f>
         <v>8918489.3000000007</v>
       </c>
-      <c r="O24" s="10">
-        <f t="shared" si="18"/>
+      <c r="O24" s="2">
+        <f>AVERAGE(G193:G202)</f>
         <v>1772.1</v>
       </c>
     </row>
@@ -2318,31 +2350,31 @@
       <c r="G25">
         <v>132</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I25" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25" s="2">
         <f>AVERAGE(B204:B213)</f>
         <v>1391121.4</v>
       </c>
-      <c r="K25" s="10">
-        <f t="shared" ref="K25:O25" si="19">AVERAGE(C204:C213)</f>
+      <c r="K25" s="2">
+        <f>AVERAGE(C204:C213)</f>
         <v>162.80000000000001</v>
       </c>
-      <c r="L25" s="10">
-        <f t="shared" si="19"/>
+      <c r="L25" s="2">
+        <f>AVERAGE(D204:D213)</f>
         <v>5370102.2000000002</v>
       </c>
-      <c r="M25" s="10">
-        <f t="shared" si="19"/>
+      <c r="M25" s="2">
+        <f>AVERAGE(E204:E213)</f>
         <v>203.6</v>
       </c>
-      <c r="N25" s="10">
-        <f t="shared" si="19"/>
+      <c r="N25" s="2">
+        <f>AVERAGE(F204:F213)</f>
         <v>8974565.3000000007</v>
       </c>
-      <c r="O25" s="10">
-        <f t="shared" si="19"/>
+      <c r="O25" s="2">
+        <f>AVERAGE(G204:G213)</f>
         <v>188.2</v>
       </c>
     </row>
@@ -2368,31 +2400,31 @@
       <c r="G26">
         <v>191</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="2">
         <f>AVERAGE(B215:B224)</f>
         <v>1271427.5</v>
       </c>
-      <c r="K26" s="10">
-        <f t="shared" ref="K26:O26" si="20">AVERAGE(C215:C224)</f>
+      <c r="K26" s="2">
+        <f>AVERAGE(C215:C224)</f>
         <v>17.100000000000001</v>
       </c>
-      <c r="L26" s="10">
-        <f t="shared" si="20"/>
+      <c r="L26" s="2">
+        <f>AVERAGE(D215:D224)</f>
         <v>994701.6</v>
       </c>
-      <c r="M26" s="10">
-        <f t="shared" si="20"/>
+      <c r="M26" s="2">
+        <f>AVERAGE(E215:E224)</f>
         <v>22.6</v>
       </c>
-      <c r="N26" s="10">
-        <f t="shared" si="20"/>
+      <c r="N26" s="2">
+        <f>AVERAGE(F215:F224)</f>
         <v>7236047.0999999996</v>
       </c>
-      <c r="O26" s="10">
-        <f t="shared" si="20"/>
+      <c r="O26" s="2">
+        <f>AVERAGE(G215:G224)</f>
         <v>20.6</v>
       </c>
     </row>
@@ -2464,6 +2496,19 @@
       <c r="G29">
         <v>386</v>
       </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="10"/>
+      <c r="L29" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M29" s="10"/>
+      <c r="N29" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O29" s="10"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -2487,6 +2532,21 @@
       <c r="G30">
         <v>448</v>
       </c>
+      <c r="I30" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="K30" s="15"/>
+      <c r="L30" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="M30" s="15"/>
+      <c r="N30" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="O30" s="15"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -2510,6 +2570,24 @@
       <c r="G31">
         <v>531</v>
       </c>
+      <c r="I31" s="11">
+        <v>1000</v>
+      </c>
+      <c r="J31" s="12">
+        <f>AVERAGE(J4:J6)</f>
+        <v>18607470.766666666</v>
+      </c>
+      <c r="K31" s="13"/>
+      <c r="L31" s="12">
+        <f t="shared" ref="L31:O31" si="8">AVERAGE(L4:L6)</f>
+        <v>435678570.76666665</v>
+      </c>
+      <c r="M31" s="13"/>
+      <c r="N31" s="12">
+        <f t="shared" ref="N31:O31" si="9">AVERAGE(N4:N6)</f>
+        <v>204068117.66666666</v>
+      </c>
+      <c r="O31" s="13"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2533,8 +2611,26 @@
       <c r="G32">
         <v>592</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32" s="11">
+        <v>100</v>
+      </c>
+      <c r="J32" s="12">
+        <f>AVERAGE(J7:J9)</f>
+        <v>1873579.3703703703</v>
+      </c>
+      <c r="K32" s="13"/>
+      <c r="L32" s="12">
+        <f t="shared" ref="L32:O32" si="10">AVERAGE(L7:L9)</f>
+        <v>24024105.551851854</v>
+      </c>
+      <c r="M32" s="13"/>
+      <c r="N32" s="12">
+        <f t="shared" ref="N32:O32" si="11">AVERAGE(N7:N9)</f>
+        <v>22307362.577777777</v>
+      </c>
+      <c r="O32" s="13"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2556,12 +2652,48 @@
       <c r="G33">
         <v>660</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" s="11">
+        <v>10</v>
+      </c>
+      <c r="J33" s="12">
+        <f>AVERAGE(J10:J13)</f>
+        <v>926885.85092592577</v>
+      </c>
+      <c r="K33" s="13"/>
+      <c r="L33" s="12">
+        <f t="shared" ref="L33:O33" si="12">AVERAGE(L10:L13)</f>
+        <v>3676263.9259259258</v>
+      </c>
+      <c r="M33" s="13"/>
+      <c r="N33" s="12">
+        <f t="shared" ref="N33:O33" si="13">AVERAGE(N10:N13)</f>
+        <v>1929087.8018518519</v>
+      </c>
+      <c r="O33" s="13"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="F34"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" s="11">
+        <v>20</v>
+      </c>
+      <c r="J34" s="12">
+        <f>AVERAGE(J17:J19)</f>
+        <v>985226.5925925927</v>
+      </c>
+      <c r="K34" s="13"/>
+      <c r="L34" s="12">
+        <f t="shared" ref="L34:O34" si="14">AVERAGE(L17:L19)</f>
+        <v>4894519.833333333</v>
+      </c>
+      <c r="M34" s="13"/>
+      <c r="N34" s="12">
+        <f t="shared" ref="N34:O34" si="15">AVERAGE(N17:N19)</f>
+        <v>2888619.7148148143</v>
+      </c>
+      <c r="O34" s="13"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2583,8 +2715,26 @@
       <c r="G35">
         <v>1420</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35" s="11">
+        <v>200</v>
+      </c>
+      <c r="J35" s="12">
+        <f>AVERAGE(J14:J16)</f>
+        <v>2919206.5185185187</v>
+      </c>
+      <c r="K35" s="13"/>
+      <c r="L35" s="12">
+        <f t="shared" ref="L35:O35" si="16">AVERAGE(L14:L16)</f>
+        <v>43000643.77407407</v>
+      </c>
+      <c r="M35" s="13"/>
+      <c r="N35" s="12">
+        <f t="shared" ref="N35:O35" si="17">AVERAGE(N14:N16)</f>
+        <v>43521172.05555556</v>
+      </c>
+      <c r="O35" s="13"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2606,8 +2756,26 @@
       <c r="G36">
         <v>1453</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36" s="11">
+        <v>50</v>
+      </c>
+      <c r="J36" s="12">
+        <f>AVERAGE(J24:J26)</f>
+        <v>1365723.9666666666</v>
+      </c>
+      <c r="K36" s="13"/>
+      <c r="L36" s="12">
+        <f t="shared" ref="L36:O36" si="18">AVERAGE(L24:L26)</f>
+        <v>13668530.566666668</v>
+      </c>
+      <c r="M36" s="13"/>
+      <c r="N36" s="12">
+        <f t="shared" ref="N36:O36" si="19">AVERAGE(N24:N26)</f>
+        <v>8376367.2333333343</v>
+      </c>
+      <c r="O36" s="13"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2629,8 +2797,26 @@
       <c r="G37">
         <v>1932</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37" s="11">
+        <v>500</v>
+      </c>
+      <c r="J37" s="12">
+        <f>AVERAGE(J20:J22)</f>
+        <v>11490133.166666666</v>
+      </c>
+      <c r="K37" s="13"/>
+      <c r="L37" s="12">
+        <f t="shared" ref="L37:O37" si="20">AVERAGE(L20:L22)</f>
+        <v>136448004.46666667</v>
+      </c>
+      <c r="M37" s="13"/>
+      <c r="N37" s="12">
+        <f t="shared" ref="N37:O37" si="21">AVERAGE(N20:N22)</f>
+        <v>105946270.63333333</v>
+      </c>
+      <c r="O37" s="13"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2653,7 +2839,7 @@
         <v>2778</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2676,7 +2862,7 @@
         <v>2855</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2699,7 +2885,7 @@
         <v>3677</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2722,7 +2908,7 @@
         <v>3884</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2745,7 +2931,7 @@
         <v>4504</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2768,7 +2954,7 @@
         <v>5713</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2791,11 +2977,11 @@
         <v>5992</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="F45"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -2818,7 +3004,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2841,7 +3027,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -6609,140 +6795,173 @@
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A232" s="11"/>
-      <c r="B232" s="11"/>
-      <c r="C232" s="11"/>
-      <c r="D232" s="11"/>
-      <c r="E232" s="11"/>
+      <c r="A232" s="3"/>
+      <c r="B232" s="3"/>
+      <c r="C232" s="3"/>
+      <c r="D232" s="3"/>
+      <c r="E232" s="3"/>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A233" s="11"/>
-      <c r="B233" s="11"/>
-      <c r="C233" s="11"/>
-      <c r="D233" s="11"/>
-      <c r="E233" s="11"/>
+      <c r="A233" s="3"/>
+      <c r="B233" s="3"/>
+      <c r="C233" s="3"/>
+      <c r="D233" s="3"/>
+      <c r="E233" s="3"/>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A234" s="11"/>
-      <c r="B234" s="11"/>
-      <c r="C234" s="11"/>
-      <c r="D234" s="11"/>
-      <c r="E234" s="11"/>
+      <c r="A234" s="3"/>
+      <c r="B234" s="3"/>
+      <c r="C234" s="3"/>
+      <c r="D234" s="3"/>
+      <c r="E234" s="3"/>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A235" s="11"/>
-      <c r="B235" s="11"/>
-      <c r="C235" s="11"/>
-      <c r="D235" s="11"/>
-      <c r="E235" s="11"/>
+      <c r="A235" s="3"/>
+      <c r="B235" s="3"/>
+      <c r="C235" s="3"/>
+      <c r="D235" s="3"/>
+      <c r="E235" s="3"/>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A236" s="11"/>
-      <c r="B236" s="11"/>
-      <c r="C236" s="11"/>
-      <c r="D236" s="11"/>
-      <c r="E236" s="11"/>
+      <c r="A236" s="3"/>
+      <c r="B236" s="3"/>
+      <c r="C236" s="3"/>
+      <c r="D236" s="3"/>
+      <c r="E236" s="3"/>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A237" s="11"/>
-      <c r="B237" s="11"/>
-      <c r="C237" s="11"/>
-      <c r="D237" s="11"/>
-      <c r="E237" s="11"/>
+      <c r="A237" s="3"/>
+      <c r="B237" s="3"/>
+      <c r="C237" s="3"/>
+      <c r="D237" s="3"/>
+      <c r="E237" s="3"/>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A238" s="11"/>
-      <c r="B238" s="11"/>
-      <c r="C238" s="11"/>
-      <c r="D238" s="11"/>
-      <c r="E238" s="11"/>
+      <c r="A238" s="3"/>
+      <c r="B238" s="3"/>
+      <c r="C238" s="3"/>
+      <c r="D238" s="3"/>
+      <c r="E238" s="3"/>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A239" s="11"/>
-      <c r="B239" s="11"/>
-      <c r="C239" s="11"/>
-      <c r="D239" s="11"/>
-      <c r="E239" s="11"/>
+      <c r="A239" s="3"/>
+      <c r="B239" s="3"/>
+      <c r="C239" s="3"/>
+      <c r="D239" s="3"/>
+      <c r="E239" s="3"/>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A240" s="11"/>
-      <c r="B240" s="11"/>
-      <c r="C240" s="11"/>
-      <c r="D240" s="11"/>
-      <c r="E240" s="11"/>
+      <c r="A240" s="3"/>
+      <c r="B240" s="3"/>
+      <c r="C240" s="3"/>
+      <c r="D240" s="3"/>
+      <c r="E240" s="3"/>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A241" s="11"/>
-      <c r="B241" s="11"/>
-      <c r="C241" s="11"/>
-      <c r="D241" s="11"/>
-      <c r="E241" s="11"/>
+      <c r="A241" s="3"/>
+      <c r="B241" s="3"/>
+      <c r="C241" s="3"/>
+      <c r="D241" s="3"/>
+      <c r="E241" s="3"/>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A242" s="11"/>
-      <c r="B242" s="11"/>
-      <c r="C242" s="11"/>
-      <c r="D242" s="11"/>
-      <c r="E242" s="11"/>
+      <c r="A242" s="3"/>
+      <c r="B242" s="3"/>
+      <c r="C242" s="3"/>
+      <c r="D242" s="3"/>
+      <c r="E242" s="3"/>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A243" s="11"/>
-      <c r="B243" s="11"/>
-      <c r="C243" s="11"/>
-      <c r="D243" s="11"/>
-      <c r="E243" s="11"/>
+      <c r="A243" s="3"/>
+      <c r="B243" s="3"/>
+      <c r="C243" s="3"/>
+      <c r="D243" s="3"/>
+      <c r="E243" s="3"/>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A244" s="11"/>
-      <c r="B244" s="11"/>
-      <c r="C244" s="11"/>
-      <c r="D244" s="11"/>
-      <c r="E244" s="11"/>
+      <c r="A244" s="3"/>
+      <c r="B244" s="3"/>
+      <c r="C244" s="3"/>
+      <c r="D244" s="3"/>
+      <c r="E244" s="3"/>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A245" s="11"/>
-      <c r="B245" s="11"/>
-      <c r="C245" s="11"/>
-      <c r="D245" s="11"/>
-      <c r="E245" s="11"/>
+      <c r="A245" s="3"/>
+      <c r="B245" s="3"/>
+      <c r="C245" s="3"/>
+      <c r="D245" s="3"/>
+      <c r="E245" s="3"/>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A246" s="11"/>
-      <c r="B246" s="11"/>
-      <c r="C246" s="11"/>
-      <c r="D246" s="11"/>
-      <c r="E246" s="11"/>
+      <c r="A246" s="3"/>
+      <c r="B246" s="3"/>
+      <c r="C246" s="3"/>
+      <c r="D246" s="3"/>
+      <c r="E246" s="3"/>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A247" s="11"/>
-      <c r="B247" s="11"/>
-      <c r="C247" s="11"/>
-      <c r="D247" s="11"/>
-      <c r="E247" s="11"/>
+      <c r="A247" s="3"/>
+      <c r="B247" s="3"/>
+      <c r="C247" s="3"/>
+      <c r="D247" s="3"/>
+      <c r="E247" s="3"/>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A248" s="11"/>
-      <c r="B248" s="11"/>
-      <c r="C248" s="11"/>
-      <c r="D248" s="11"/>
-      <c r="E248" s="11"/>
+      <c r="A248" s="3"/>
+      <c r="B248" s="3"/>
+      <c r="C248" s="3"/>
+      <c r="D248" s="3"/>
+      <c r="E248" s="3"/>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A249" s="11"/>
-      <c r="B249" s="11"/>
-      <c r="C249" s="11"/>
-      <c r="D249" s="11"/>
-      <c r="E249" s="11"/>
+      <c r="A249" s="3"/>
+      <c r="B249" s="3"/>
+      <c r="C249" s="3"/>
+      <c r="D249" s="3"/>
+      <c r="E249" s="3"/>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A250" s="11"/>
-      <c r="B250" s="11"/>
-      <c r="C250" s="11"/>
-      <c r="D250" s="11"/>
-      <c r="E250" s="11"/>
+      <c r="A250" s="3"/>
+      <c r="B250" s="3"/>
+      <c r="C250" s="3"/>
+      <c r="D250" s="3"/>
+      <c r="E250" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="I19 I26" twoDigitTextYear="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
tableau pour partie 1 et deux
miawmiawmiwamw
</commit_message>
<xml_diff>
--- a/tp2/logs/donnees.xlsx
+++ b/tp2/logs/donnees.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gravu_000\Documents\GitHub\INF4705\tp2\logs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="23715" windowHeight="9270"/>
   </bookViews>
@@ -19,7 +14,7 @@
   <definedNames>
     <definedName name="analyse_1" localSheetId="0">Feuil1!$A$1:$G$224</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -42,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="250">
   <si>
     <t>Nom du fichier</t>
   </si>
@@ -756,6 +751,42 @@
   </si>
   <si>
     <t>Temps(ns)</t>
+  </si>
+  <si>
+    <t>meilleur</t>
+  </si>
+  <si>
+    <t>pire</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>capacité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taille </t>
+  </si>
+  <si>
+    <t>y/f(x)</t>
   </si>
 </sst>
 </file>
@@ -813,7 +844,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -875,11 +906,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -901,12 +954,6 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -922,6 +969,21 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -944,7 +1006,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -986,7 +1048,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1021,7 +1083,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1230,13 +1292,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O250"/>
+  <dimension ref="A1:AA250"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
@@ -1253,7 +1315,7 @@
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1276,7 +1338,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1301,20 +1363,36 @@
       <c r="I2" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="9" t="s">
+      <c r="K2" s="15"/>
+      <c r="L2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="9" t="s">
+      <c r="M2" s="15"/>
+      <c r="N2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="10"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O2" s="15"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" s="18"/>
+      <c r="X2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1355,8 +1433,44 @@
       <c r="O3" s="6" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="AA3" s="19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1405,8 +1519,54 @@
         <f t="shared" si="0"/>
         <v>32469.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>1000</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="R4" s="1" t="str">
+        <f>Q4</f>
+        <v>1000</v>
+      </c>
+      <c r="S4" s="20">
+        <f>J4/R4</f>
+        <v>19172.238100000002</v>
+      </c>
+      <c r="T4" s="1">
+        <f>Q4^2</f>
+        <v>1000000</v>
+      </c>
+      <c r="U4" s="1">
+        <f>J4/T4</f>
+        <v>19.172238100000001</v>
+      </c>
+      <c r="V4" s="1">
+        <f>Q4*P4</f>
+        <v>1000000</v>
+      </c>
+      <c r="W4" s="1">
+        <f>L4/(V4)</f>
+        <v>1109.4751162999999</v>
+      </c>
+      <c r="X4" s="1" t="str">
+        <f>Q4</f>
+        <v>1000</v>
+      </c>
+      <c r="Y4" s="1">
+        <f>N4/X4</f>
+        <v>220425.56890000001</v>
+      </c>
+      <c r="Z4" s="1">
+        <f>Q4^2</f>
+        <v>1000000</v>
+      </c>
+      <c r="AA4" s="1">
+        <f>N4/Z4</f>
+        <v>220.4255689</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1455,8 +1615,54 @@
         <f t="shared" si="1"/>
         <v>3335.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>1000</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="R5" s="1" t="str">
+        <f t="shared" ref="R5:R24" si="2">Q5</f>
+        <v>500</v>
+      </c>
+      <c r="S5" s="20">
+        <f t="shared" ref="S5:S24" si="3">J5/R5</f>
+        <v>34165.625999999997</v>
+      </c>
+      <c r="T5" s="1">
+        <f t="shared" ref="T5:T24" si="4">Q5^2</f>
+        <v>250000</v>
+      </c>
+      <c r="U5" s="1">
+        <f t="shared" ref="U5:U24" si="5">J5/T5</f>
+        <v>68.331252000000006</v>
+      </c>
+      <c r="V5" s="1">
+        <f t="shared" ref="V5:V24" si="6">Q5*P5</f>
+        <v>500000</v>
+      </c>
+      <c r="W5" s="1">
+        <f t="shared" ref="W5:W24" si="7">L5/(V5)</f>
+        <v>295.46784980000001</v>
+      </c>
+      <c r="X5" s="1" t="str">
+        <f t="shared" ref="X5:X24" si="8">Q5</f>
+        <v>500</v>
+      </c>
+      <c r="Y5" s="1">
+        <f t="shared" ref="Y5:Y24" si="9">N5/X5</f>
+        <v>408410.68400000001</v>
+      </c>
+      <c r="Z5" s="1">
+        <f t="shared" ref="Z5:Z24" si="10">Q5^2</f>
+        <v>250000</v>
+      </c>
+      <c r="AA5" s="1">
+        <f t="shared" ref="AA5:AA24" si="11">N5/Z5</f>
+        <v>816.82136800000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1486,27 +1692,73 @@
         <v>19567361.199999999</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" ref="K6:O6" si="2">AVERAGE(C24:C33)</f>
+        <f t="shared" ref="K6:O6" si="12">AVERAGE(C24:C33)</f>
         <v>313.89999999999998</v>
       </c>
       <c r="L6" s="2">
+        <f t="shared" si="12"/>
+        <v>49826671.100000001</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="12"/>
+        <v>421</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="12"/>
+        <v>187573442.09999999</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="12"/>
+        <v>360.3</v>
+      </c>
+      <c r="P6">
+        <v>1000</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="R6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>49826671.100000001</v>
-      </c>
-      <c r="M6" s="2">
-        <f t="shared" si="2"/>
-        <v>421</v>
-      </c>
-      <c r="N6" s="2">
-        <f t="shared" si="2"/>
-        <v>187573442.09999999</v>
-      </c>
-      <c r="O6" s="2">
-        <f t="shared" si="2"/>
-        <v>360.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="S6" s="20">
+        <f t="shared" si="3"/>
+        <v>97836.805999999997</v>
+      </c>
+      <c r="T6" s="1">
+        <f t="shared" si="4"/>
+        <v>40000</v>
+      </c>
+      <c r="U6" s="1">
+        <f t="shared" si="5"/>
+        <v>489.18403000000001</v>
+      </c>
+      <c r="V6" s="1">
+        <f t="shared" si="6"/>
+        <v>200000</v>
+      </c>
+      <c r="W6" s="1">
+        <f t="shared" si="7"/>
+        <v>249.13335549999999</v>
+      </c>
+      <c r="X6" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>200</v>
+      </c>
+      <c r="Y6" s="1">
+        <f t="shared" si="9"/>
+        <v>937867.21049999993</v>
+      </c>
+      <c r="Z6" s="1">
+        <f t="shared" si="10"/>
+        <v>40000</v>
+      </c>
+      <c r="AA6" s="1">
+        <f t="shared" si="11"/>
+        <v>4689.3360524999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1536,27 +1788,73 @@
         <v>1929205</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" ref="K7:O7" si="3">AVERAGE(C35:C44)</f>
+        <f t="shared" ref="K7:O7" si="13">AVERAGE(C35:C44)</f>
         <v>2859.5</v>
       </c>
       <c r="L7" s="2">
+        <f t="shared" si="13"/>
+        <v>52673413.100000001</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="13"/>
+        <v>3675.7</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="13"/>
+        <v>24649228.399999999</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="13"/>
+        <v>3420.8</v>
+      </c>
+      <c r="P7">
+        <v>1000</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="R7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="S7" s="20">
         <f t="shared" si="3"/>
-        <v>52673413.100000001</v>
-      </c>
-      <c r="M7" s="2">
-        <f t="shared" si="3"/>
-        <v>3675.7</v>
-      </c>
-      <c r="N7" s="2">
-        <f t="shared" si="3"/>
-        <v>24649228.399999999</v>
-      </c>
-      <c r="O7" s="2">
-        <f t="shared" si="3"/>
-        <v>3420.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>19292.05</v>
+      </c>
+      <c r="T7" s="1">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="U7" s="1">
+        <f t="shared" si="5"/>
+        <v>192.9205</v>
+      </c>
+      <c r="V7" s="1">
+        <f t="shared" si="6"/>
+        <v>100000</v>
+      </c>
+      <c r="W7" s="1">
+        <f t="shared" si="7"/>
+        <v>526.73413100000005</v>
+      </c>
+      <c r="X7" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="Y7" s="1">
+        <f t="shared" si="9"/>
+        <v>246492.28399999999</v>
+      </c>
+      <c r="Z7" s="1">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+      <c r="AA7" s="1">
+        <f t="shared" si="11"/>
+        <v>2464.9228399999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1586,27 +1884,73 @@
         <v>1942892.2222222222</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" ref="K8:O8" si="4">AVERAGE(C46:C54)</f>
+        <f t="shared" ref="K8:O8" si="14">AVERAGE(C46:C54)</f>
         <v>315.66666666666669</v>
       </c>
       <c r="L8" s="2">
+        <f t="shared" si="14"/>
+        <v>17472890.666666668</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="14"/>
+        <v>403.66666666666669</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="14"/>
+        <v>25056521.111111112</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="14"/>
+        <v>369.88888888888891</v>
+      </c>
+      <c r="P8">
+        <v>1000</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="R8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="S8" s="20">
+        <f t="shared" si="3"/>
+        <v>38857.844444444447</v>
+      </c>
+      <c r="T8" s="1">
         <f t="shared" si="4"/>
-        <v>17472890.666666668</v>
-      </c>
-      <c r="M8" s="2">
-        <f t="shared" si="4"/>
-        <v>403.66666666666669</v>
-      </c>
-      <c r="N8" s="2">
-        <f t="shared" si="4"/>
-        <v>25056521.111111112</v>
-      </c>
-      <c r="O8" s="2">
-        <f t="shared" si="4"/>
-        <v>369.88888888888891</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2500</v>
+      </c>
+      <c r="U8" s="1">
+        <f t="shared" si="5"/>
+        <v>777.15688888888894</v>
+      </c>
+      <c r="V8" s="1">
+        <f t="shared" si="6"/>
+        <v>50000</v>
+      </c>
+      <c r="W8" s="1">
+        <f t="shared" si="7"/>
+        <v>349.45781333333338</v>
+      </c>
+      <c r="X8" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="Y8" s="1">
+        <f t="shared" si="9"/>
+        <v>501130.42222222226</v>
+      </c>
+      <c r="Z8" s="1">
+        <f t="shared" si="10"/>
+        <v>2500</v>
+      </c>
+      <c r="AA8" s="1">
+        <f t="shared" si="11"/>
+        <v>10022.608444444444</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1636,27 +1980,73 @@
         <v>1748640.888888889</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" ref="K9:O9" si="5">AVERAGE(C56:C64)</f>
+        <f t="shared" ref="K9:O9" si="15">AVERAGE(C56:C64)</f>
         <v>32.666666666666664</v>
       </c>
       <c r="L9" s="2">
+        <f t="shared" si="15"/>
+        <v>1926012.888888889</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="15"/>
+        <v>43.333333333333336</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="15"/>
+        <v>17216338.222222224</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="15"/>
+        <v>39</v>
+      </c>
+      <c r="P9">
+        <v>1000</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="R9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="S9" s="20">
+        <f t="shared" si="3"/>
+        <v>87432.044444444444</v>
+      </c>
+      <c r="T9" s="1">
+        <f t="shared" si="4"/>
+        <v>400</v>
+      </c>
+      <c r="U9" s="1">
         <f t="shared" si="5"/>
-        <v>1926012.888888889</v>
-      </c>
-      <c r="M9" s="2">
-        <f t="shared" si="5"/>
-        <v>43.333333333333336</v>
-      </c>
-      <c r="N9" s="2">
-        <f t="shared" si="5"/>
-        <v>17216338.222222224</v>
-      </c>
-      <c r="O9" s="2">
-        <f t="shared" si="5"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>4371.6022222222227</v>
+      </c>
+      <c r="V9" s="1">
+        <f t="shared" si="6"/>
+        <v>20000</v>
+      </c>
+      <c r="W9" s="1">
+        <f t="shared" si="7"/>
+        <v>96.300644444444444</v>
+      </c>
+      <c r="X9" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="Y9" s="1">
+        <f t="shared" si="9"/>
+        <v>860816.91111111117</v>
+      </c>
+      <c r="Z9" s="1">
+        <f t="shared" si="10"/>
+        <v>400</v>
+      </c>
+      <c r="AA9" s="1">
+        <f t="shared" si="11"/>
+        <v>43040.845555555563</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1686,27 +2076,73 @@
         <v>910659.875</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" ref="K10:O10" si="6">AVERAGE(C66:C73)</f>
+        <f t="shared" ref="K10:O10" si="16">AVERAGE(C66:C73)</f>
         <v>1004.75</v>
       </c>
       <c r="L10" s="2">
+        <f t="shared" si="16"/>
+        <v>9498412.5</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="16"/>
+        <v>1106.125</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="16"/>
+        <v>1939351.75</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="16"/>
+        <v>1069.375</v>
+      </c>
+      <c r="P10">
+        <v>1000</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="R10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="S10" s="20">
+        <f t="shared" si="3"/>
+        <v>91065.987500000003</v>
+      </c>
+      <c r="T10" s="1">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="U10" s="1">
+        <f t="shared" si="5"/>
+        <v>9106.5987499999992</v>
+      </c>
+      <c r="V10" s="1">
         <f t="shared" si="6"/>
-        <v>9498412.5</v>
-      </c>
-      <c r="M10" s="2">
-        <f t="shared" si="6"/>
-        <v>1106.125</v>
-      </c>
-      <c r="N10" s="2">
-        <f t="shared" si="6"/>
-        <v>1939351.75</v>
-      </c>
-      <c r="O10" s="2">
-        <f t="shared" si="6"/>
-        <v>1069.375</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="W10" s="1">
+        <f t="shared" si="7"/>
+        <v>949.84124999999995</v>
+      </c>
+      <c r="X10" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="Y10" s="1">
+        <f t="shared" si="9"/>
+        <v>193935.17499999999</v>
+      </c>
+      <c r="Z10" s="1">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="AA10" s="1">
+        <f t="shared" si="11"/>
+        <v>19393.517500000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1736,38 +2172,150 @@
         <v>955876.9</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" ref="K11:O11" si="7">AVERAGE(C75:C84)</f>
+        <f t="shared" ref="K11:O11" si="17">AVERAGE(C75:C84)</f>
         <v>89.1</v>
       </c>
       <c r="L11" s="2">
+        <f t="shared" si="17"/>
+        <v>918119.5</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="17"/>
+        <v>108.2</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="17"/>
+        <v>1929649.1</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="17"/>
+        <v>99.6</v>
+      </c>
+      <c r="P11">
+        <v>100</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="R11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="S11" s="20">
+        <f t="shared" si="3"/>
+        <v>955.87689999999998</v>
+      </c>
+      <c r="T11" s="1">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="U11" s="1">
+        <f t="shared" si="5"/>
+        <v>0.95587690000000003</v>
+      </c>
+      <c r="V11" s="1">
+        <f t="shared" si="6"/>
+        <v>100000</v>
+      </c>
+      <c r="W11" s="1">
         <f t="shared" si="7"/>
-        <v>918119.5</v>
-      </c>
-      <c r="M11" s="2">
-        <f t="shared" si="7"/>
-        <v>108.2</v>
-      </c>
-      <c r="N11" s="2">
-        <f t="shared" si="7"/>
-        <v>1929649.1</v>
-      </c>
-      <c r="O11" s="2">
-        <f t="shared" si="7"/>
-        <v>99.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9.1811950000000007</v>
+      </c>
+      <c r="X11" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>1000</v>
+      </c>
+      <c r="Y11" s="1">
+        <f t="shared" si="9"/>
+        <v>1929.6491000000001</v>
+      </c>
+      <c r="Z11" s="1">
+        <f t="shared" si="10"/>
+        <v>1000000</v>
+      </c>
+      <c r="AA11" s="1">
+        <f t="shared" si="11"/>
+        <v>1.9296491</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="F12"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I12" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="J12" s="2">
+        <f>AVERAGE(B86:B94)</f>
+        <v>914120.77777777775</v>
+      </c>
+      <c r="K12" s="2">
+        <f>AVERAGE(C86:C94)</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="L12" s="2">
+        <f>AVERAGE(D86:D94)</f>
+        <v>612259.77777777775</v>
+      </c>
+      <c r="M12" s="2">
+        <f>AVERAGE(E86:E94)</f>
+        <v>13.111111111111111</v>
+      </c>
+      <c r="N12" s="2">
+        <f>AVERAGE(F86:F94)</f>
+        <v>1918262.5555555555</v>
+      </c>
+      <c r="O12" s="2">
+        <f>AVERAGE(G86:G94)</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="P12">
+        <v>100</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="R12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="S12" s="20">
+        <f t="shared" si="3"/>
+        <v>1828.2415555555556</v>
+      </c>
+      <c r="T12" s="1">
+        <f t="shared" si="4"/>
+        <v>250000</v>
+      </c>
+      <c r="U12" s="1">
+        <f t="shared" si="5"/>
+        <v>3.6564831111111111</v>
+      </c>
+      <c r="V12" s="1">
+        <f t="shared" si="6"/>
+        <v>50000</v>
+      </c>
+      <c r="W12" s="1">
+        <f t="shared" si="7"/>
+        <v>12.245195555555554</v>
+      </c>
+      <c r="X12" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>500</v>
+      </c>
+      <c r="Y12" s="1">
+        <f t="shared" si="9"/>
+        <v>3836.5251111111111</v>
+      </c>
+      <c r="Z12" s="1">
+        <f t="shared" si="10"/>
+        <v>250000</v>
+      </c>
+      <c r="AA12" s="1">
+        <f t="shared" si="11"/>
+        <v>7.6730502222222219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1790,34 +2338,80 @@
         <v>664</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J13" s="2">
-        <f>AVERAGE(B86:B94)</f>
-        <v>914120.77777777775</v>
+        <f>AVERAGE(B96:B104)</f>
+        <v>3114161.5555555555</v>
       </c>
       <c r="K13" s="2">
-        <f>AVERAGE(C86:C94)</f>
-        <v>11.111111111111111</v>
+        <f>AVERAGE(C96:C104)</f>
+        <v>5891.1111111111113</v>
       </c>
       <c r="L13" s="2">
-        <f>AVERAGE(D86:D94)</f>
-        <v>612259.77777777775</v>
+        <f>AVERAGE(D96:D104)</f>
+        <v>77868910.222222224</v>
       </c>
       <c r="M13" s="2">
-        <f>AVERAGE(E86:E94)</f>
-        <v>13.111111111111111</v>
+        <f>AVERAGE(E96:E104)</f>
+        <v>7610.7777777777774</v>
       </c>
       <c r="N13" s="2">
-        <f>AVERAGE(F86:F94)</f>
-        <v>1918262.5555555555</v>
+        <f>AVERAGE(F96:F104)</f>
+        <v>46580486.666666664</v>
       </c>
       <c r="O13" s="2">
-        <f>AVERAGE(G86:G94)</f>
-        <v>11.333333333333334</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <f>AVERAGE(G96:G104)</f>
+        <v>6884.2222222222226</v>
+      </c>
+      <c r="P13">
+        <v>100</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="R13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="S13" s="20">
+        <f t="shared" si="3"/>
+        <v>15570.807777777778</v>
+      </c>
+      <c r="T13" s="1">
+        <f t="shared" si="4"/>
+        <v>40000</v>
+      </c>
+      <c r="U13" s="1">
+        <f t="shared" si="5"/>
+        <v>77.854038888888894</v>
+      </c>
+      <c r="V13" s="1">
+        <f t="shared" si="6"/>
+        <v>20000</v>
+      </c>
+      <c r="W13" s="1">
+        <f t="shared" si="7"/>
+        <v>3893.445511111111</v>
+      </c>
+      <c r="X13" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>200</v>
+      </c>
+      <c r="Y13" s="1">
+        <f t="shared" si="9"/>
+        <v>232902.43333333332</v>
+      </c>
+      <c r="Z13" s="1">
+        <f t="shared" si="10"/>
+        <v>40000</v>
+      </c>
+      <c r="AA13" s="1">
+        <f t="shared" si="11"/>
+        <v>1164.5121666666666</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1840,34 +2434,80 @@
         <v>1254</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="J14" s="2">
-        <f>AVERAGE(B96:B104)</f>
-        <v>3114161.5555555555</v>
+        <f>AVERAGE(B106:B115)</f>
+        <v>2918555.8</v>
       </c>
       <c r="K14" s="2">
-        <f>AVERAGE(C96:C104)</f>
-        <v>5891.1111111111113</v>
+        <f>AVERAGE(C106:C115)</f>
+        <v>574.9</v>
       </c>
       <c r="L14" s="2">
-        <f>AVERAGE(D96:D104)</f>
-        <v>77868910.222222224</v>
+        <f>AVERAGE(D106:D115)</f>
+        <v>41854789.799999997</v>
       </c>
       <c r="M14" s="2">
-        <f>AVERAGE(E96:E104)</f>
-        <v>7610.7777777777774</v>
+        <f>AVERAGE(E106:E115)</f>
+        <v>741</v>
       </c>
       <c r="N14" s="2">
-        <f>AVERAGE(F96:F104)</f>
-        <v>46580486.666666664</v>
+        <f>AVERAGE(F106:F115)</f>
+        <v>45450803.700000003</v>
       </c>
       <c r="O14" s="2">
-        <f>AVERAGE(G96:G104)</f>
-        <v>6884.2222222222226</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <f>AVERAGE(G106:G115)</f>
+        <v>678.5</v>
+      </c>
+      <c r="P14">
+        <v>100</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="R14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="S14" s="20">
+        <f t="shared" si="3"/>
+        <v>29185.557999999997</v>
+      </c>
+      <c r="T14" s="1">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="U14" s="1">
+        <f t="shared" si="5"/>
+        <v>291.85557999999997</v>
+      </c>
+      <c r="V14" s="1">
+        <f t="shared" si="6"/>
+        <v>10000</v>
+      </c>
+      <c r="W14" s="1">
+        <f t="shared" si="7"/>
+        <v>4185.4789799999999</v>
+      </c>
+      <c r="X14" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="Y14" s="1">
+        <f t="shared" si="9"/>
+        <v>454508.03700000001</v>
+      </c>
+      <c r="Z14" s="1">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+      <c r="AA14" s="1">
+        <f t="shared" si="11"/>
+        <v>4545.0803700000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1890,34 +2530,80 @@
         <v>1793</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J15" s="2">
-        <f>AVERAGE(B106:B115)</f>
-        <v>2918555.8</v>
+        <f>AVERAGE(B117:B126)</f>
+        <v>2724902.2</v>
       </c>
       <c r="K15" s="2">
-        <f>AVERAGE(C106:C115)</f>
-        <v>574.9</v>
+        <f>AVERAGE(C117:C126)</f>
+        <v>62.5</v>
       </c>
       <c r="L15" s="2">
-        <f>AVERAGE(D106:D115)</f>
-        <v>41854789.799999997</v>
+        <f>AVERAGE(D117:D126)</f>
+        <v>9278231.3000000007</v>
       </c>
       <c r="M15" s="2">
-        <f>AVERAGE(E106:E115)</f>
-        <v>741</v>
+        <f>AVERAGE(E117:E126)</f>
+        <v>83.8</v>
       </c>
       <c r="N15" s="2">
-        <f>AVERAGE(F106:F115)</f>
-        <v>45450803.700000003</v>
+        <f>AVERAGE(F117:F126)</f>
+        <v>38532225.799999997</v>
       </c>
       <c r="O15" s="2">
-        <f>AVERAGE(G106:G115)</f>
-        <v>678.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <f>AVERAGE(G117:G126)</f>
+        <v>73.8</v>
+      </c>
+      <c r="P15">
+        <v>100</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="R15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="S15" s="20">
+        <f t="shared" si="3"/>
+        <v>54498.044000000002</v>
+      </c>
+      <c r="T15" s="1">
+        <f t="shared" si="4"/>
+        <v>2500</v>
+      </c>
+      <c r="U15" s="1">
+        <f t="shared" si="5"/>
+        <v>1089.9608800000001</v>
+      </c>
+      <c r="V15" s="1">
+        <f t="shared" si="6"/>
+        <v>5000</v>
+      </c>
+      <c r="W15" s="1">
+        <f t="shared" si="7"/>
+        <v>1855.6462600000002</v>
+      </c>
+      <c r="X15" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="Y15" s="1">
+        <f t="shared" si="9"/>
+        <v>770644.51599999995</v>
+      </c>
+      <c r="Z15" s="1">
+        <f t="shared" si="10"/>
+        <v>2500</v>
+      </c>
+      <c r="AA15" s="1">
+        <f t="shared" si="11"/>
+        <v>15412.890319999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1940,34 +2626,80 @@
         <v>2426</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J16" s="2">
-        <f>AVERAGE(B117:B126)</f>
-        <v>2724902.2</v>
+        <f>AVERAGE(B128:B136)</f>
+        <v>1002141.7777777778</v>
       </c>
       <c r="K16" s="2">
-        <f>AVERAGE(C117:C126)</f>
-        <v>62.5</v>
+        <f>AVERAGE(C128:C136)</f>
+        <v>967.11111111111109</v>
       </c>
       <c r="L16" s="2">
-        <f>AVERAGE(D117:D126)</f>
-        <v>9278231.3000000007</v>
+        <f>AVERAGE(D128:D136)</f>
+        <v>12751036</v>
       </c>
       <c r="M16" s="2">
-        <f>AVERAGE(E117:E126)</f>
-        <v>83.8</v>
+        <f>AVERAGE(E128:E136)</f>
+        <v>1235.5555555555557</v>
       </c>
       <c r="N16" s="2">
-        <f>AVERAGE(F117:F126)</f>
-        <v>38532225.799999997</v>
+        <f>AVERAGE(F128:F136)</f>
+        <v>3018903.4444444445</v>
       </c>
       <c r="O16" s="2">
-        <f>AVERAGE(G117:G126)</f>
-        <v>73.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <f>AVERAGE(G128:G136)</f>
+        <v>1101.7777777777778</v>
+      </c>
+      <c r="P16">
+        <v>100</v>
+      </c>
+      <c r="Q16" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="R16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="S16" s="20">
+        <f t="shared" si="3"/>
+        <v>50107.088888888888</v>
+      </c>
+      <c r="T16" s="1">
+        <f t="shared" si="4"/>
+        <v>400</v>
+      </c>
+      <c r="U16" s="1">
+        <f t="shared" si="5"/>
+        <v>2505.3544444444442</v>
+      </c>
+      <c r="V16" s="1">
+        <f t="shared" si="6"/>
+        <v>2000</v>
+      </c>
+      <c r="W16" s="1">
+        <f t="shared" si="7"/>
+        <v>6375.518</v>
+      </c>
+      <c r="X16" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="Y16" s="1">
+        <f t="shared" si="9"/>
+        <v>150945.17222222223</v>
+      </c>
+      <c r="Z16" s="1">
+        <f t="shared" si="10"/>
+        <v>400</v>
+      </c>
+      <c r="AA16" s="1">
+        <f t="shared" si="11"/>
+        <v>7547.2586111111113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1990,34 +2722,80 @@
         <v>3015</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="J17" s="2">
-        <f>AVERAGE(B128:B136)</f>
-        <v>1002141.7777777778</v>
+        <f>AVERAGE(B138:B147)</f>
+        <v>1008420.7</v>
       </c>
       <c r="K17" s="2">
-        <f>AVERAGE(C128:C136)</f>
-        <v>967.11111111111109</v>
+        <f>AVERAGE(C138:C147)</f>
+        <v>99.2</v>
       </c>
       <c r="L17" s="2">
-        <f>AVERAGE(D128:D136)</f>
-        <v>12751036</v>
+        <f>AVERAGE(D138:D147)</f>
+        <v>1267146.3</v>
       </c>
       <c r="M17" s="2">
-        <f>AVERAGE(E128:E136)</f>
-        <v>1235.5555555555557</v>
+        <f>AVERAGE(E138:E147)</f>
+        <v>119.9</v>
       </c>
       <c r="N17" s="2">
-        <f>AVERAGE(F128:F136)</f>
-        <v>3018903.4444444445</v>
+        <f>AVERAGE(F138:F147)</f>
+        <v>2839615.4</v>
       </c>
       <c r="O17" s="2">
-        <f>AVERAGE(G128:G136)</f>
-        <v>1101.7777777777778</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <f>AVERAGE(G138:G147)</f>
+        <v>111.1</v>
+      </c>
+      <c r="P17">
+        <v>100</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="R17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="S17" s="20">
+        <f t="shared" si="3"/>
+        <v>100842.06999999999</v>
+      </c>
+      <c r="T17" s="1">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="U17" s="1">
+        <f t="shared" si="5"/>
+        <v>10084.207</v>
+      </c>
+      <c r="V17" s="1">
+        <f t="shared" si="6"/>
+        <v>1000</v>
+      </c>
+      <c r="W17" s="1">
+        <f t="shared" si="7"/>
+        <v>1267.1463000000001</v>
+      </c>
+      <c r="X17" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="Y17" s="1">
+        <f t="shared" si="9"/>
+        <v>283961.53999999998</v>
+      </c>
+      <c r="Z17" s="1">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="AA17" s="1">
+        <f t="shared" si="11"/>
+        <v>28396.153999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2040,34 +2818,80 @@
         <v>3645</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J18" s="2">
-        <f>AVERAGE(B138:B147)</f>
-        <v>1008420.7</v>
+        <f>AVERAGE(B149:B158)</f>
+        <v>945117.3</v>
       </c>
       <c r="K18" s="2">
-        <f>AVERAGE(C138:C147)</f>
-        <v>99.2</v>
+        <f>AVERAGE(C149:C158)</f>
+        <v>11.7</v>
       </c>
       <c r="L18" s="2">
-        <f>AVERAGE(D138:D147)</f>
-        <v>1267146.3</v>
+        <f>AVERAGE(D149:D158)</f>
+        <v>665377.19999999995</v>
       </c>
       <c r="M18" s="2">
-        <f>AVERAGE(E138:E147)</f>
-        <v>119.9</v>
+        <f>AVERAGE(E149:E158)</f>
+        <v>13.9</v>
       </c>
       <c r="N18" s="2">
-        <f>AVERAGE(F138:F147)</f>
-        <v>2839615.4</v>
+        <f>AVERAGE(F149:F158)</f>
+        <v>2807340.3</v>
       </c>
       <c r="O18" s="2">
-        <f>AVERAGE(G138:G147)</f>
-        <v>111.1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <f>AVERAGE(G149:G158)</f>
+        <v>13</v>
+      </c>
+      <c r="P18">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="R18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="S18" s="20">
+        <f t="shared" si="3"/>
+        <v>945.1173</v>
+      </c>
+      <c r="T18" s="1">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="U18" s="1">
+        <f t="shared" si="5"/>
+        <v>0.94511730000000005</v>
+      </c>
+      <c r="V18" s="1">
+        <f t="shared" si="6"/>
+        <v>10000</v>
+      </c>
+      <c r="W18" s="1">
+        <f t="shared" si="7"/>
+        <v>66.537719999999993</v>
+      </c>
+      <c r="X18" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>1000</v>
+      </c>
+      <c r="Y18" s="1">
+        <f t="shared" si="9"/>
+        <v>2807.3402999999998</v>
+      </c>
+      <c r="Z18" s="1">
+        <f t="shared" si="10"/>
+        <v>1000000</v>
+      </c>
+      <c r="AA18" s="1">
+        <f t="shared" si="11"/>
+        <v>2.8073402999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2090,34 +2914,80 @@
         <v>4150</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="J19" s="2">
-        <f>AVERAGE(B149:B158)</f>
-        <v>945117.3</v>
+        <f>AVERAGE(B160:B169)</f>
+        <v>12165247.300000001</v>
       </c>
       <c r="K19" s="2">
-        <f>AVERAGE(C149:C158)</f>
-        <v>11.7</v>
+        <f>AVERAGE(C160:C169)</f>
+        <v>13751.8</v>
       </c>
       <c r="L19" s="2">
-        <f>AVERAGE(D149:D158)</f>
-        <v>665377.19999999995</v>
+        <f>AVERAGE(D160:D169)</f>
+        <v>309694953.39999998</v>
       </c>
       <c r="M19" s="2">
-        <f>AVERAGE(E149:E158)</f>
-        <v>13.9</v>
+        <f>AVERAGE(E160:E169)</f>
+        <v>18027.2</v>
       </c>
       <c r="N19" s="2">
-        <f>AVERAGE(F149:F158)</f>
-        <v>2807340.3</v>
+        <f>AVERAGE(F160:F169)</f>
+        <v>114938772</v>
       </c>
       <c r="O19" s="2">
-        <f>AVERAGE(G149:G158)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <f>AVERAGE(G160:G169)</f>
+        <v>16239.8</v>
+      </c>
+      <c r="P19">
+        <v>10</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="R19" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="S19" s="20">
+        <f t="shared" si="3"/>
+        <v>24330.494600000002</v>
+      </c>
+      <c r="T19" s="1">
+        <f t="shared" si="4"/>
+        <v>250000</v>
+      </c>
+      <c r="U19" s="1">
+        <f t="shared" si="5"/>
+        <v>48.660989200000003</v>
+      </c>
+      <c r="V19" s="1">
+        <f t="shared" si="6"/>
+        <v>5000</v>
+      </c>
+      <c r="W19" s="1">
+        <f t="shared" si="7"/>
+        <v>61938.990679999995</v>
+      </c>
+      <c r="X19" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>500</v>
+      </c>
+      <c r="Y19" s="1">
+        <f t="shared" si="9"/>
+        <v>229877.54399999999</v>
+      </c>
+      <c r="Z19" s="1">
+        <f t="shared" si="10"/>
+        <v>250000</v>
+      </c>
+      <c r="AA19" s="1">
+        <f t="shared" si="11"/>
+        <v>459.755088</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -2140,34 +3010,80 @@
         <v>4927</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="J20" s="2">
-        <f>AVERAGE(B160:B169)</f>
-        <v>12165247.300000001</v>
+        <f>AVERAGE(B171:B180)</f>
+        <v>11623733.800000001</v>
       </c>
       <c r="K20" s="2">
-        <f>AVERAGE(C160:C169)</f>
-        <v>13751.8</v>
+        <f>AVERAGE(C171:C180)</f>
+        <v>1429.5</v>
       </c>
       <c r="L20" s="2">
-        <f>AVERAGE(D160:D169)</f>
-        <v>309694953.39999998</v>
+        <f>AVERAGE(D171:D180)</f>
+        <v>64749464.799999997</v>
       </c>
       <c r="M20" s="2">
-        <f>AVERAGE(E160:E169)</f>
-        <v>18027.2</v>
+        <f>AVERAGE(E171:E180)</f>
+        <v>1858.8</v>
       </c>
       <c r="N20" s="2">
-        <f>AVERAGE(F160:F169)</f>
-        <v>114938772</v>
+        <f>AVERAGE(F171:F180)</f>
+        <v>104298181.7</v>
       </c>
       <c r="O20" s="2">
-        <f>AVERAGE(G160:G169)</f>
-        <v>16239.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <f>AVERAGE(G171:G180)</f>
+        <v>1676</v>
+      </c>
+      <c r="P20">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="R20" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="S20" s="20">
+        <f t="shared" si="3"/>
+        <v>58118.669000000002</v>
+      </c>
+      <c r="T20" s="1">
+        <f t="shared" si="4"/>
+        <v>40000</v>
+      </c>
+      <c r="U20" s="1">
+        <f t="shared" si="5"/>
+        <v>290.593345</v>
+      </c>
+      <c r="V20" s="1">
+        <f t="shared" si="6"/>
+        <v>2000</v>
+      </c>
+      <c r="W20" s="1">
+        <f t="shared" si="7"/>
+        <v>32374.732399999997</v>
+      </c>
+      <c r="X20" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>200</v>
+      </c>
+      <c r="Y20" s="1">
+        <f t="shared" si="9"/>
+        <v>521490.90850000002</v>
+      </c>
+      <c r="Z20" s="1">
+        <f t="shared" si="10"/>
+        <v>40000</v>
+      </c>
+      <c r="AA20" s="1">
+        <f t="shared" si="11"/>
+        <v>2607.4545425000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2190,34 +3106,80 @@
         <v>5469</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J21" s="2">
-        <f>AVERAGE(B171:B180)</f>
-        <v>11623733.800000001</v>
+        <f>AVERAGE(B182:B191)</f>
+        <v>10681418.4</v>
       </c>
       <c r="K21" s="2">
-        <f>AVERAGE(C171:C180)</f>
-        <v>1429.5</v>
+        <f>AVERAGE(C182:C191)</f>
+        <v>153.80000000000001</v>
       </c>
       <c r="L21" s="2">
-        <f>AVERAGE(D171:D180)</f>
-        <v>64749464.799999997</v>
+        <f>AVERAGE(D182:D191)</f>
+        <v>34899595.200000003</v>
       </c>
       <c r="M21" s="2">
-        <f>AVERAGE(E171:E180)</f>
-        <v>1858.8</v>
+        <f>AVERAGE(E182:E191)</f>
+        <v>209.5</v>
       </c>
       <c r="N21" s="2">
-        <f>AVERAGE(F171:F180)</f>
-        <v>104298181.7</v>
+        <f>AVERAGE(F182:F191)</f>
+        <v>98601858.200000003</v>
       </c>
       <c r="O21" s="2">
-        <f>AVERAGE(G171:G180)</f>
-        <v>1676</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <f>AVERAGE(G182:G191)</f>
+        <v>181.6</v>
+      </c>
+      <c r="P21">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="R21" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="S21" s="20">
+        <f t="shared" si="3"/>
+        <v>106814.18400000001</v>
+      </c>
+      <c r="T21" s="1">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="U21" s="1">
+        <f t="shared" si="5"/>
+        <v>1068.14184</v>
+      </c>
+      <c r="V21" s="1">
+        <f t="shared" si="6"/>
+        <v>1000</v>
+      </c>
+      <c r="W21" s="1">
+        <f t="shared" si="7"/>
+        <v>34899.595200000003</v>
+      </c>
+      <c r="X21" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="Y21" s="1">
+        <f t="shared" si="9"/>
+        <v>986018.58200000005</v>
+      </c>
+      <c r="Z21" s="1">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+      <c r="AA21" s="1">
+        <f t="shared" si="11"/>
+        <v>9860.1858200000006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2240,45 +3202,157 @@
         <v>6014</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J22" s="2">
-        <f>AVERAGE(B182:B191)</f>
-        <v>10681418.4</v>
+        <f>AVERAGE(B193:B202)</f>
+        <v>1434623</v>
       </c>
       <c r="K22" s="2">
-        <f>AVERAGE(C182:C191)</f>
-        <v>153.80000000000001</v>
+        <f>AVERAGE(C193:C202)</f>
+        <v>1629.1</v>
       </c>
       <c r="L22" s="2">
-        <f>AVERAGE(D182:D191)</f>
-        <v>34899595.200000003</v>
+        <f>AVERAGE(D193:D202)</f>
+        <v>34640787.899999999</v>
       </c>
       <c r="M22" s="2">
-        <f>AVERAGE(E182:E191)</f>
-        <v>209.5</v>
+        <f>AVERAGE(E193:E202)</f>
+        <v>1967.6</v>
       </c>
       <c r="N22" s="2">
-        <f>AVERAGE(F182:F191)</f>
-        <v>98601858.200000003</v>
+        <f>AVERAGE(F193:F202)</f>
+        <v>8918489.3000000007</v>
       </c>
       <c r="O22" s="2">
-        <f>AVERAGE(G182:G191)</f>
-        <v>181.6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <f>AVERAGE(G193:G202)</f>
+        <v>1772.1</v>
+      </c>
+      <c r="P22">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="R22" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="S22" s="20">
+        <f t="shared" si="3"/>
+        <v>28692.46</v>
+      </c>
+      <c r="T22" s="1">
+        <f t="shared" si="4"/>
+        <v>2500</v>
+      </c>
+      <c r="U22" s="1">
+        <f t="shared" si="5"/>
+        <v>573.8492</v>
+      </c>
+      <c r="V22" s="1">
+        <f t="shared" si="6"/>
+        <v>500</v>
+      </c>
+      <c r="W22" s="1">
+        <f t="shared" si="7"/>
+        <v>69281.575799999991</v>
+      </c>
+      <c r="X22" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="Y22" s="1">
+        <f t="shared" si="9"/>
+        <v>178369.78600000002</v>
+      </c>
+      <c r="Z22" s="1">
+        <f t="shared" si="10"/>
+        <v>2500</v>
+      </c>
+      <c r="AA22" s="1">
+        <f t="shared" si="11"/>
+        <v>3567.3957200000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="F23"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I23" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="J23" s="2">
+        <f>AVERAGE(B204:B213)</f>
+        <v>1391121.4</v>
+      </c>
+      <c r="K23" s="2">
+        <f>AVERAGE(C204:C213)</f>
+        <v>162.80000000000001</v>
+      </c>
+      <c r="L23" s="2">
+        <f>AVERAGE(D204:D213)</f>
+        <v>5370102.2000000002</v>
+      </c>
+      <c r="M23" s="2">
+        <f>AVERAGE(E204:E213)</f>
+        <v>203.6</v>
+      </c>
+      <c r="N23" s="2">
+        <f>AVERAGE(F204:F213)</f>
+        <v>8974565.3000000007</v>
+      </c>
+      <c r="O23" s="2">
+        <f>AVERAGE(G204:G213)</f>
+        <v>188.2</v>
+      </c>
+      <c r="P23">
+        <v>10</v>
+      </c>
+      <c r="Q23" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="R23" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="S23" s="20">
+        <f t="shared" si="3"/>
+        <v>69556.069999999992</v>
+      </c>
+      <c r="T23" s="1">
+        <f t="shared" si="4"/>
+        <v>400</v>
+      </c>
+      <c r="U23" s="1">
+        <f t="shared" si="5"/>
+        <v>3477.8035</v>
+      </c>
+      <c r="V23" s="1">
+        <f t="shared" si="6"/>
+        <v>200</v>
+      </c>
+      <c r="W23" s="1">
+        <f t="shared" si="7"/>
+        <v>26850.511000000002</v>
+      </c>
+      <c r="X23" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="Y23" s="1">
+        <f t="shared" si="9"/>
+        <v>448728.26500000001</v>
+      </c>
+      <c r="Z23" s="1">
+        <f t="shared" si="10"/>
+        <v>400</v>
+      </c>
+      <c r="AA23" s="1">
+        <f t="shared" si="11"/>
+        <v>22436.413250000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2301,34 +3375,80 @@
         <v>67</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="J24" s="2">
-        <f>AVERAGE(B193:B202)</f>
-        <v>1434623</v>
+        <f>AVERAGE(B215:B224)</f>
+        <v>1271427.5</v>
       </c>
       <c r="K24" s="2">
-        <f>AVERAGE(C193:C202)</f>
-        <v>1629.1</v>
+        <f>AVERAGE(C215:C224)</f>
+        <v>17.100000000000001</v>
       </c>
       <c r="L24" s="2">
-        <f>AVERAGE(D193:D202)</f>
-        <v>34640787.899999999</v>
+        <f>AVERAGE(D215:D224)</f>
+        <v>994701.6</v>
       </c>
       <c r="M24" s="2">
-        <f>AVERAGE(E193:E202)</f>
-        <v>1967.6</v>
+        <f>AVERAGE(E215:E224)</f>
+        <v>22.6</v>
       </c>
       <c r="N24" s="2">
-        <f>AVERAGE(F193:F202)</f>
-        <v>8918489.3000000007</v>
+        <f>AVERAGE(F215:F224)</f>
+        <v>7236047.0999999996</v>
       </c>
       <c r="O24" s="2">
-        <f>AVERAGE(G193:G202)</f>
-        <v>1772.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+        <f>AVERAGE(G215:G224)</f>
+        <v>20.6</v>
+      </c>
+      <c r="P24">
+        <v>10</v>
+      </c>
+      <c r="Q24" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="R24" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="S24" s="20">
+        <f t="shared" si="3"/>
+        <v>127142.75</v>
+      </c>
+      <c r="T24" s="1">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="U24" s="1">
+        <f t="shared" si="5"/>
+        <v>12714.275</v>
+      </c>
+      <c r="V24" s="1">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="W24" s="1">
+        <f t="shared" si="7"/>
+        <v>9947.0159999999996</v>
+      </c>
+      <c r="X24" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="Y24" s="1">
+        <f t="shared" si="9"/>
+        <v>723604.71</v>
+      </c>
+      <c r="Z24" s="1">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="AA24" s="1">
+        <f t="shared" si="11"/>
+        <v>72360.47099999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2350,35 +3470,8 @@
       <c r="G25">
         <v>132</v>
       </c>
-      <c r="I25" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="J25" s="2">
-        <f>AVERAGE(B204:B213)</f>
-        <v>1391121.4</v>
-      </c>
-      <c r="K25" s="2">
-        <f>AVERAGE(C204:C213)</f>
-        <v>162.80000000000001</v>
-      </c>
-      <c r="L25" s="2">
-        <f>AVERAGE(D204:D213)</f>
-        <v>5370102.2000000002</v>
-      </c>
-      <c r="M25" s="2">
-        <f>AVERAGE(E204:E213)</f>
-        <v>203.6</v>
-      </c>
-      <c r="N25" s="2">
-        <f>AVERAGE(F204:F213)</f>
-        <v>8974565.3000000007</v>
-      </c>
-      <c r="O25" s="2">
-        <f>AVERAGE(G204:G213)</f>
-        <v>188.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2400,35 +3493,8 @@
       <c r="G26">
         <v>191</v>
       </c>
-      <c r="I26" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="J26" s="2">
-        <f>AVERAGE(B215:B224)</f>
-        <v>1271427.5</v>
-      </c>
-      <c r="K26" s="2">
-        <f>AVERAGE(C215:C224)</f>
-        <v>17.100000000000001</v>
-      </c>
-      <c r="L26" s="2">
-        <f>AVERAGE(D215:D224)</f>
-        <v>994701.6</v>
-      </c>
-      <c r="M26" s="2">
-        <f>AVERAGE(E215:E224)</f>
-        <v>22.6</v>
-      </c>
-      <c r="N26" s="2">
-        <f>AVERAGE(F215:F224)</f>
-        <v>7236047.0999999996</v>
-      </c>
-      <c r="O26" s="2">
-        <f>AVERAGE(G215:G224)</f>
-        <v>20.6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2451,7 +3517,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2474,7 +3540,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2497,20 +3563,20 @@
         <v>386</v>
       </c>
       <c r="I29" s="8"/>
-      <c r="J29" s="9" t="s">
+      <c r="J29" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="K29" s="10"/>
-      <c r="L29" s="9" t="s">
+      <c r="K29" s="15"/>
+      <c r="L29" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="M29" s="10"/>
-      <c r="N29" s="9" t="s">
+      <c r="M29" s="15"/>
+      <c r="N29" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O29" s="10"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O29" s="15"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2535,20 +3601,20 @@
       <c r="I30" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="J30" s="14" t="s">
+      <c r="J30" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="K30" s="15"/>
-      <c r="L30" s="14" t="s">
+      <c r="K30" s="13"/>
+      <c r="L30" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="M30" s="15"/>
-      <c r="N30" s="14" t="s">
+      <c r="M30" s="13"/>
+      <c r="N30" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="O30" s="15"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O30" s="13"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2570,26 +3636,26 @@
       <c r="G31">
         <v>531</v>
       </c>
-      <c r="I31" s="11">
+      <c r="I31" s="9">
         <v>1000</v>
       </c>
-      <c r="J31" s="12">
+      <c r="J31" s="10">
         <f>AVERAGE(J4:J6)</f>
         <v>18607470.766666666</v>
       </c>
-      <c r="K31" s="13"/>
-      <c r="L31" s="12">
-        <f t="shared" ref="L31:O31" si="8">AVERAGE(L4:L6)</f>
+      <c r="K31" s="11"/>
+      <c r="L31" s="10">
+        <f>AVERAGE(L4:L6)</f>
         <v>435678570.76666665</v>
       </c>
-      <c r="M31" s="13"/>
-      <c r="N31" s="12">
-        <f t="shared" ref="N31:O31" si="9">AVERAGE(N4:N6)</f>
+      <c r="M31" s="11"/>
+      <c r="N31" s="10">
+        <f>AVERAGE(N4:N6)</f>
         <v>204068117.66666666</v>
       </c>
-      <c r="O31" s="13"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O31" s="11"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2611,24 +3677,24 @@
       <c r="G32">
         <v>592</v>
       </c>
-      <c r="I32" s="11">
+      <c r="I32" s="9">
         <v>100</v>
       </c>
-      <c r="J32" s="12">
+      <c r="J32" s="10">
         <f>AVERAGE(J7:J9)</f>
         <v>1873579.3703703703</v>
       </c>
-      <c r="K32" s="13"/>
-      <c r="L32" s="12">
-        <f t="shared" ref="L32:O32" si="10">AVERAGE(L7:L9)</f>
+      <c r="K32" s="11"/>
+      <c r="L32" s="10">
+        <f>AVERAGE(L7:L9)</f>
         <v>24024105.551851854</v>
       </c>
-      <c r="M32" s="13"/>
-      <c r="N32" s="12">
-        <f t="shared" ref="N32:O32" si="11">AVERAGE(N7:N9)</f>
+      <c r="M32" s="11"/>
+      <c r="N32" s="10">
+        <f>AVERAGE(N7:N9)</f>
         <v>22307362.577777777</v>
       </c>
-      <c r="O32" s="13"/>
+      <c r="O32" s="11"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -2652,46 +3718,46 @@
       <c r="G33">
         <v>660</v>
       </c>
-      <c r="I33" s="11">
+      <c r="I33" s="9">
         <v>10</v>
       </c>
-      <c r="J33" s="12">
-        <f>AVERAGE(J10:J13)</f>
+      <c r="J33" s="10">
+        <f>AVERAGE(J10:J12)</f>
         <v>926885.85092592577</v>
       </c>
-      <c r="K33" s="13"/>
-      <c r="L33" s="12">
-        <f t="shared" ref="L33:O33" si="12">AVERAGE(L10:L13)</f>
+      <c r="K33" s="11"/>
+      <c r="L33" s="10">
+        <f>AVERAGE(L10:L12)</f>
         <v>3676263.9259259258</v>
       </c>
-      <c r="M33" s="13"/>
-      <c r="N33" s="12">
-        <f t="shared" ref="N33:O33" si="13">AVERAGE(N10:N13)</f>
+      <c r="M33" s="11"/>
+      <c r="N33" s="10">
+        <f>AVERAGE(N10:N12)</f>
         <v>1929087.8018518519</v>
       </c>
-      <c r="O33" s="13"/>
+      <c r="O33" s="11"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="F34"/>
-      <c r="I34" s="11">
+      <c r="I34" s="9">
         <v>20</v>
       </c>
-      <c r="J34" s="12">
-        <f>AVERAGE(J17:J19)</f>
+      <c r="J34" s="10">
+        <f>AVERAGE(J16:J18)</f>
         <v>985226.5925925927</v>
       </c>
-      <c r="K34" s="13"/>
-      <c r="L34" s="12">
-        <f t="shared" ref="L34:O34" si="14">AVERAGE(L17:L19)</f>
+      <c r="K34" s="11"/>
+      <c r="L34" s="10">
+        <f>AVERAGE(L16:L18)</f>
         <v>4894519.833333333</v>
       </c>
-      <c r="M34" s="13"/>
-      <c r="N34" s="12">
-        <f t="shared" ref="N34:O34" si="15">AVERAGE(N17:N19)</f>
+      <c r="M34" s="11"/>
+      <c r="N34" s="10">
+        <f>AVERAGE(N16:N18)</f>
         <v>2888619.7148148143</v>
       </c>
-      <c r="O34" s="13"/>
+      <c r="O34" s="11"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -2715,24 +3781,24 @@
       <c r="G35">
         <v>1420</v>
       </c>
-      <c r="I35" s="11">
+      <c r="I35" s="9">
         <v>200</v>
       </c>
-      <c r="J35" s="12">
-        <f>AVERAGE(J14:J16)</f>
+      <c r="J35" s="10">
+        <f>AVERAGE(J13:J15)</f>
         <v>2919206.5185185187</v>
       </c>
-      <c r="K35" s="13"/>
-      <c r="L35" s="12">
-        <f t="shared" ref="L35:O35" si="16">AVERAGE(L14:L16)</f>
+      <c r="K35" s="11"/>
+      <c r="L35" s="10">
+        <f>AVERAGE(L13:L15)</f>
         <v>43000643.77407407</v>
       </c>
-      <c r="M35" s="13"/>
-      <c r="N35" s="12">
-        <f t="shared" ref="N35:O35" si="17">AVERAGE(N14:N16)</f>
+      <c r="M35" s="11"/>
+      <c r="N35" s="10">
+        <f>AVERAGE(N13:N15)</f>
         <v>43521172.05555556</v>
       </c>
-      <c r="O35" s="13"/>
+      <c r="O35" s="11"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -2756,24 +3822,24 @@
       <c r="G36">
         <v>1453</v>
       </c>
-      <c r="I36" s="11">
+      <c r="I36" s="9">
         <v>50</v>
       </c>
-      <c r="J36" s="12">
-        <f>AVERAGE(J24:J26)</f>
+      <c r="J36" s="10">
+        <f>AVERAGE(J22:J24)</f>
         <v>1365723.9666666666</v>
       </c>
-      <c r="K36" s="13"/>
-      <c r="L36" s="12">
-        <f t="shared" ref="L36:O36" si="18">AVERAGE(L24:L26)</f>
+      <c r="K36" s="11"/>
+      <c r="L36" s="10">
+        <f>AVERAGE(L22:L24)</f>
         <v>13668530.566666668</v>
       </c>
-      <c r="M36" s="13"/>
-      <c r="N36" s="12">
-        <f t="shared" ref="N36:O36" si="19">AVERAGE(N24:N26)</f>
+      <c r="M36" s="11"/>
+      <c r="N36" s="10">
+        <f>AVERAGE(N22:N24)</f>
         <v>8376367.2333333343</v>
       </c>
-      <c r="O36" s="13"/>
+      <c r="O36" s="11"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -2797,24 +3863,24 @@
       <c r="G37">
         <v>1932</v>
       </c>
-      <c r="I37" s="11">
+      <c r="I37" s="9">
         <v>500</v>
       </c>
-      <c r="J37" s="12">
-        <f>AVERAGE(J20:J22)</f>
+      <c r="J37" s="10">
+        <f>AVERAGE(J19:J21)</f>
         <v>11490133.166666666</v>
       </c>
-      <c r="K37" s="13"/>
-      <c r="L37" s="12">
-        <f t="shared" ref="L37:O37" si="20">AVERAGE(L20:L22)</f>
+      <c r="K37" s="11"/>
+      <c r="L37" s="10">
+        <f>AVERAGE(L19:L21)</f>
         <v>136448004.46666667</v>
       </c>
-      <c r="M37" s="13"/>
-      <c r="N37" s="12">
-        <f t="shared" ref="N37:O37" si="21">AVERAGE(N20:N22)</f>
+      <c r="M37" s="11"/>
+      <c r="N37" s="10">
+        <f>AVERAGE(N19:N21)</f>
         <v>105946270.63333333</v>
       </c>
-      <c r="O37" s="13"/>
+      <c r="O37" s="11"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -6929,42 +7995,39 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="L30:M30"/>
     <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="L29:M29"/>
     <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
     <mergeCell ref="N29:O29"/>
     <mergeCell ref="J31:K31"/>
     <mergeCell ref="J32:K32"/>
     <mergeCell ref="J33:K33"/>
     <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="L37:M37"/>
     <mergeCell ref="J35:K35"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J37:K37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="I19 I26" twoDigitTextYear="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -6974,7 +8037,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6986,7 +8049,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>